<commit_message>
Jenkins API Test and Result added
</commit_message>
<xml_diff>
--- a/src/test/java/ExcelFiles/LoginInfo.xlsx
+++ b/src/test/java/ExcelFiles/LoginInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="8490" windowHeight="7590" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>turkeyts</t>
+    <t>username</t>
   </si>
   <si>
-    <t>TechnoStudy123</t>
+    <t>password</t>
   </si>
   <si>
     <t>invalidUser</t>
@@ -963,12 +963,13 @@
   <sheetPr/>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
+    <col min="1" max="1" width="12.5714285714286" customWidth="1"/>
     <col min="2" max="2" width="17.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="11.8571428571429" customWidth="1"/>
   </cols>
@@ -992,8 +993,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>